<commit_message>
Update SIR with rate units
</commit_message>
<xml_diff>
--- a/atomica/library/sir_databook.xlsx
+++ b/atomica/library/sir_databook.xlsx
@@ -1,473 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8424CD2D-04CE-4BAF-97BC-AB6B0E80A59C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4D9BCA-87DF-459B-B921-EB786B98D7B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1596" yWindow="318" windowWidth="17280" windowHeight="7686" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="State Variables" sheetId="2" r:id="rId2"/>
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>None</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column is for the abbreviated name of a population.
-It is only ever used as a reference label within the code.
-Note: It should be in lower case without spaces.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column is for the full name of a population.
-It will appear in plots and analysis outputs.
-Note: It should be in title or sentence case.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>None</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column defines a 'label' attribute for a 'comp' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a characteristic.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a characteristic.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>None</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -475,58 +40,76 @@
     <t>Full Name</t>
   </si>
   <si>
+    <t>Population type</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Susceptible</t>
+  </si>
+  <si>
+    <t>Provenance</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Uncertainty</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Total number of entities</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>Transmission probability per contact</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Framework-supplied default</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Number of contacts annually</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>Average duration of infections (years)</t>
+  </si>
+  <si>
+    <t>Duration (years)</t>
+  </si>
+  <si>
+    <t>Death rate for infected people</t>
+  </si>
+  <si>
+    <t>Rate (per year)</t>
+  </si>
+  <si>
+    <t>Death rate for susceptible people</t>
+  </si>
+  <si>
     <t>adults</t>
   </si>
   <si>
     <t>Adults</t>
-  </si>
-  <si>
-    <t>Susceptible</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>Total number of entities</t>
-  </si>
-  <si>
-    <t>Prevalence</t>
-  </si>
-  <si>
-    <t>Fraction</t>
-  </si>
-  <si>
-    <t>Transmission probability per contact</t>
-  </si>
-  <si>
-    <t>Probability</t>
-  </si>
-  <si>
-    <t>Number of contacts annually</t>
-  </si>
-  <si>
-    <t>N.A.</t>
-  </si>
-  <si>
-    <t>Average duration of infections (years)</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Death rate for infected people</t>
-  </si>
-  <si>
-    <t>Death rate for susceptible people</t>
   </si>
 </sst>
 </file>
@@ -550,15 +133,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98E0FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -566,15 +161,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,7 +211,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -915,56 +605,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="14.83984375" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.15625" customWidth="1"/>
+    <col min="2" max="2" width="12.68359375" customWidth="1"/>
+    <col min="3" max="3" width="10.578125" customWidth="1"/>
+    <col min="4" max="4" width="13.83984375" customWidth="1"/>
+    <col min="5" max="23" width="9.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -974,6 +678,9 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E1" s="1">
         <v>2000</v>
       </c>
@@ -1032,17 +739,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="3"/>
       <c r="E2">
         <v>700</v>
       </c>
@@ -1101,7 +806,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1111,6 +816,9 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="1">
         <v>2000</v>
       </c>
@@ -1169,17 +877,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="3"/>
       <c r="E5">
         <v>1000</v>
       </c>
@@ -1238,7 +944,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1248,6 +954,9 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="1">
         <v>2000</v>
       </c>
@@ -1306,17 +1015,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8">
         <v>0.28571428999999998</v>
       </c>
@@ -1377,34 +1084,40 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Fraction"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF808080"/>
+  </sheetPr>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.578125" customWidth="1"/>
+    <col min="2" max="2" width="30.26171875" customWidth="1"/>
+    <col min="3" max="3" width="19.26171875" customWidth="1"/>
+    <col min="4" max="4" width="13.83984375" customWidth="1"/>
+    <col min="5" max="5" width="10.578125" customWidth="1"/>
+    <col min="6" max="6" width="3.83984375" customWidth="1"/>
+    <col min="7" max="25" width="9.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1414,82 +1127,112 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1">
         <v>2000</v>
       </c>
-      <c r="F1" s="1">
+      <c r="H1" s="1">
         <v>2001</v>
       </c>
-      <c r="G1" s="1">
+      <c r="I1" s="1">
         <v>2002</v>
       </c>
-      <c r="H1" s="1">
+      <c r="J1" s="1">
         <v>2003</v>
       </c>
-      <c r="I1" s="1">
+      <c r="K1" s="1">
         <v>2004</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L1" s="1">
         <v>2005</v>
       </c>
-      <c r="K1" s="1">
+      <c r="M1" s="1">
         <v>2006</v>
       </c>
-      <c r="L1" s="1">
+      <c r="N1" s="1">
         <v>2007</v>
       </c>
-      <c r="M1" s="1">
+      <c r="O1" s="1">
         <v>2008</v>
       </c>
-      <c r="N1" s="1">
+      <c r="P1" s="1">
         <v>2009</v>
       </c>
-      <c r="O1" s="1">
+      <c r="Q1" s="1">
         <v>2010</v>
       </c>
-      <c r="P1" s="1">
+      <c r="R1" s="1">
         <v>2011</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="S1" s="1">
         <v>2012</v>
       </c>
-      <c r="R1" s="1">
+      <c r="T1" s="1">
         <v>2013</v>
       </c>
-      <c r="S1" s="1">
+      <c r="U1" s="1">
         <v>2014</v>
       </c>
-      <c r="T1" s="1">
+      <c r="V1" s="1">
         <v>2015</v>
       </c>
-      <c r="U1" s="1">
+      <c r="W1" s="1">
         <v>2016</v>
       </c>
-      <c r="V1" s="1">
+      <c r="X1" s="1">
         <v>2017</v>
       </c>
-      <c r="W1" s="1">
+      <c r="Y1" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1497,83 +1240,112 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>2000</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>2001</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>2002</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>2003</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>2004</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>2005</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>2006</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>2007</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>2008</v>
       </c>
-      <c r="N4" s="1">
+      <c r="P4" s="1">
         <v>2009</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>2010</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>2011</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="S4" s="1">
         <v>2012</v>
       </c>
-      <c r="R4" s="1">
+      <c r="T4" s="1">
         <v>2013</v>
       </c>
-      <c r="S4" s="1">
+      <c r="U4" s="1">
         <v>2014</v>
       </c>
-      <c r="T4" s="1">
+      <c r="V4" s="1">
         <v>2015</v>
       </c>
-      <c r="U4" s="1">
+      <c r="W4" s="1">
         <v>2016</v>
       </c>
-      <c r="V4" s="1">
+      <c r="X4" s="1">
         <v>2017</v>
       </c>
-      <c r="W4" s="1">
+      <c r="Y4" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <f>IF(SUMPRODUCT(--(E5:W5&lt;&gt;""))=0,80,"N.A.")</f>
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>80</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1581,82 +1353,112 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
         <v>2000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>2001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I7" s="1">
         <v>2002</v>
       </c>
-      <c r="H7" s="1">
+      <c r="J7" s="1">
         <v>2003</v>
       </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
         <v>2004</v>
       </c>
-      <c r="J7" s="1">
+      <c r="L7" s="1">
         <v>2005</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>2006</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <v>2007</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <v>2008</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <v>2009</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <v>2010</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>2011</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="S7" s="1">
         <v>2012</v>
       </c>
-      <c r="R7" s="1">
+      <c r="T7" s="1">
         <v>2013</v>
       </c>
-      <c r="S7" s="1">
+      <c r="U7" s="1">
         <v>2014</v>
       </c>
-      <c r="T7" s="1">
+      <c r="V7" s="1">
         <v>2015</v>
       </c>
-      <c r="U7" s="1">
+      <c r="W7" s="1">
         <v>2016</v>
       </c>
-      <c r="V7" s="1">
+      <c r="X7" s="1">
         <v>2017</v>
       </c>
-      <c r="W7" s="1">
+      <c r="Y7" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -1664,83 +1466,112 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="1">
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
         <v>2000</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>2001</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
         <v>2002</v>
       </c>
-      <c r="H10" s="1">
+      <c r="J10" s="1">
         <v>2003</v>
       </c>
-      <c r="I10" s="1">
+      <c r="K10" s="1">
         <v>2004</v>
       </c>
-      <c r="J10" s="1">
+      <c r="L10" s="1">
         <v>2005</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
         <v>2006</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1">
         <v>2007</v>
       </c>
-      <c r="M10" s="1">
+      <c r="O10" s="1">
         <v>2008</v>
       </c>
-      <c r="N10" s="1">
+      <c r="P10" s="1">
         <v>2009</v>
       </c>
-      <c r="O10" s="1">
+      <c r="Q10" s="1">
         <v>2010</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>2011</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="S10" s="1">
         <v>2012</v>
       </c>
-      <c r="R10" s="1">
+      <c r="T10" s="1">
         <v>2013</v>
       </c>
-      <c r="S10" s="1">
+      <c r="U10" s="1">
         <v>2014</v>
       </c>
-      <c r="T10" s="1">
+      <c r="V10" s="1">
         <v>2015</v>
       </c>
-      <c r="U10" s="1">
+      <c r="W10" s="1">
         <v>2016</v>
       </c>
-      <c r="V10" s="1">
+      <c r="X10" s="1">
         <v>2017</v>
       </c>
-      <c r="W10" s="1">
+      <c r="Y10" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <f>IF(SUMPRODUCT(--(E11:W11&lt;&gt;""))=0,0.016,"N.A.")</f>
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <v>1.6E-2</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1748,90 +1579,164 @@
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="1">
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
         <v>2000</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>2001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <v>2002</v>
       </c>
-      <c r="H13" s="1">
+      <c r="J13" s="1">
         <v>2003</v>
       </c>
-      <c r="I13" s="1">
+      <c r="K13" s="1">
         <v>2004</v>
       </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1">
         <v>2005</v>
       </c>
-      <c r="K13" s="1">
+      <c r="M13" s="1">
         <v>2006</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1">
         <v>2007</v>
       </c>
-      <c r="M13" s="1">
+      <c r="O13" s="1">
         <v>2008</v>
       </c>
-      <c r="N13" s="1">
+      <c r="P13" s="1">
         <v>2009</v>
       </c>
-      <c r="O13" s="1">
+      <c r="Q13" s="1">
         <v>2010</v>
       </c>
-      <c r="P13" s="1">
+      <c r="R13" s="1">
         <v>2011</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="S13" s="1">
         <v>2012</v>
       </c>
-      <c r="R13" s="1">
+      <c r="T13" s="1">
         <v>2013</v>
       </c>
-      <c r="S13" s="1">
+      <c r="U13" s="1">
         <v>2014</v>
       </c>
-      <c r="T13" s="1">
+      <c r="V13" s="1">
         <v>2015</v>
       </c>
-      <c r="U13" s="1">
+      <c r="W13" s="1">
         <v>2016</v>
       </c>
-      <c r="V13" s="1">
+      <c r="X13" s="1">
         <v>2017</v>
       </c>
-      <c r="W13" s="1">
+      <c r="Y13" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="str">
-        <f>'Population Definitions'!A2</f>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14">
-        <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,0.008,"N.A.")</f>
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B14 B2 B11" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>COUNTIF(G11:Y11,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>AND(COUNTIF(G11:Y11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>COUNTIF(G14:Y14,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>AND(COUNTIF(G14:Y14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>COUNTIF(G2:Y2,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>AND(COUNTIF(G2:Y2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>COUNTIF(G5:Y5,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND(COUNTIF(G5:Y5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>COUNTIF(G8:Y8,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>AND(COUNTIF(G8:Y8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>"Duration"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0200-000002000000}">
+      <formula1>"Duration (years)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C14" xr:uid="{00000000-0002-0000-0200-000003000000}">
+      <formula1>"Rate (per year)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>